<commit_message>
Tamir zamani validasyon, servise verilis tarihi otomatik doldur, tedarikci otomatik sec
</commit_message>
<xml_diff>
--- a/data/belgrad/BEL25_FRACAS(Hata Raporlama Analizi ve Düzeltici Aksiyon Sitemi) Formu - 2025.12.3 S.xlsx
+++ b/data/belgrad/BEL25_FRACAS(Hata Raporlama Analizi ve Düzeltici Aksiyon Sitemi) Formu - 2025.12.3 S.xlsx
@@ -24594,20 +24594,24 @@
       </c>
     </row>
     <row r="161">
-      <c r="D161" t="inlineStr"/>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>15000</t>
+        </is>
+      </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>BEL25-036</t>
+          <t>BEL25-037</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>Tahrik Konvertörü Sis. Aux ekipmanı</t>
+          <t>Tahrik Konvertörü Sis.  Fan Sistemi</t>
         </is>
       </c>
       <c r="I161" t="inlineStr">
@@ -24617,21 +24621,34 @@
       </c>
       <c r="J161" t="inlineStr">
         <is>
-          <t>adadad</t>
+          <t>arıza tamir</t>
         </is>
       </c>
       <c r="K161" t="inlineStr">
         <is>
-          <t>Yüksek</t>
+          <t>A-Kritik/Emniyet Riski</t>
         </is>
       </c>
       <c r="L161" t="inlineStr">
         <is>
-          <t>Kullanıcı Hatası</t>
+          <t>Müşteri</t>
         </is>
       </c>
-      <c r="M161" t="inlineStr"/>
-      <c r="N161" t="inlineStr"/>
+      <c r="M161" t="inlineStr">
+        <is>
+          <t>müdahale</t>
+        </is>
+      </c>
+      <c r="N161" t="inlineStr">
+        <is>
+          <t>Tamir</t>
+        </is>
+      </c>
+      <c r="O161" t="inlineStr">
+        <is>
+          <t>Evet</t>
+        </is>
+      </c>
       <c r="Q161" t="inlineStr">
         <is>
           <t>2026-02-02</t>
@@ -24639,7 +24656,7 @@
       </c>
       <c r="R161" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="U161" t="inlineStr">
@@ -24647,8 +24664,16 @@
           <t>Elektrik</t>
         </is>
       </c>
-      <c r="X161" t="inlineStr"/>
-      <c r="Z161" t="inlineStr"/>
+      <c r="X161" t="inlineStr">
+        <is>
+          <t>G420-7798</t>
+        </is>
+      </c>
+      <c r="Z161" t="inlineStr">
+        <is>
+          <t>TAVAN SACI (PASLANMAZ)</t>
+        </is>
+      </c>
       <c r="AA161" t="inlineStr">
         <is>
           <t>1</t>

</xml_diff>